<commit_message>
Cleric spells and archetype feats Refactoring notes
</commit_message>
<xml_diff>
--- a/wornitems.xlsx
+++ b/wornitems.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1352" documentId="11_87BB4F5ABF64FF18F55B1250EA3161BAE35CC59B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E8E314F-8629-4C6F-AAA4-7253F4411327}"/>
+  <xr:revisionPtr revIDLastSave="1379" documentId="11_87BB4F5ABF64FF18F55B1250EA3161BAE35CC59B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE0A949A-C930-47BB-8B63-F2B9123C3E59}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="38310" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work" sheetId="2" r:id="rId1"/>
     <sheet name="Transposed CSV export" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Work!$C$1:$IA$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Work!$C$1:$IA$144</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5240" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5239" uniqueCount="1125">
   <si>
     <t>desc</t>
   </si>
@@ -3408,15 +3408,31 @@
   </si>
   <si>
     <t>19cde2df-4421-4d01-a898-51d57d41787c</t>
+  </si>
+  <si>
+    <t>This bright red-and-gold cape is often interlaced with glittery threads and serves as a distraction. While wearing the cape, you gain a +2 item bonus to Deception checks.</t>
+  </si>
+  <si>
+    <t>You cast dimension door. The space you leave and the one you appear in are filled with puffs of smoke that make anyone within concealed until they leave the smoke or the end of your next turn, at which point the smoke dissipates. Strong winds immediately disperse the smoke.</t>
+  </si>
+  <si>
+    <t>Dimension Door</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3603,88 +3619,95 @@
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="10" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="10" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="7" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="9" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="13" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="13" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -3702,7 +3725,17 @@
     <cellStyle name="60% - Accent4" xfId="10" builtinId="44"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3841,29 +3874,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4272,13 +4285,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FF1657-1808-4FD3-8283-EF1F402CCA42}">
-  <dimension ref="A1:IA159"/>
+  <dimension ref="A1:IA157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B127" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="X70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A147" sqref="A147"/>
+      <selection pane="bottomRight" activeCell="X80" sqref="X80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5398,7 +5411,7 @@
       <c r="ED2" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="EE2" s="8" t="s">
+      <c r="EE2" s="73" t="s">
         <v>844</v>
       </c>
       <c r="EF2" s="8" t="s">
@@ -5922,6 +5935,9 @@
       <c r="ED3" s="9" t="s">
         <v>269</v>
       </c>
+      <c r="EE3" s="67" t="s">
+        <v>1122</v>
+      </c>
       <c r="EG3" s="9" t="s">
         <v>555</v>
       </c>
@@ -10745,6 +10761,9 @@
       <c r="ED19" s="10" t="s">
         <v>275</v>
       </c>
+      <c r="EE19" s="10" t="s">
+        <v>204</v>
+      </c>
       <c r="EG19" s="10" t="s">
         <v>204</v>
       </c>
@@ -11516,6 +11535,9 @@
       <c r="DR42" s="63" t="s">
         <v>218</v>
       </c>
+      <c r="EE42" s="68" t="s">
+        <v>948</v>
+      </c>
       <c r="EH42" s="63" t="s">
         <v>389</v>
       </c>
@@ -11629,6 +11651,9 @@
       <c r="DR43" s="6" t="s">
         <v>173</v>
       </c>
+      <c r="EE43" s="69" t="s">
+        <v>173</v>
+      </c>
       <c r="EH43" s="6" t="s">
         <v>173</v>
       </c>
@@ -11736,6 +11761,9 @@
       <c r="DR44" s="6" t="s">
         <v>209</v>
       </c>
+      <c r="EE44" s="6">
+        <v>2</v>
+      </c>
       <c r="EH44" s="6">
         <v>2</v>
       </c>
@@ -11993,6 +12021,9 @@
       <c r="ED54" s="64" t="s">
         <v>271</v>
       </c>
+      <c r="EE54" s="70" t="s">
+        <v>676</v>
+      </c>
       <c r="EG54" s="64" t="s">
         <v>563</v>
       </c>
@@ -12139,6 +12170,9 @@
       <c r="ED55" s="4" t="s">
         <v>270</v>
       </c>
+      <c r="EE55" s="4" t="s">
+        <v>844</v>
+      </c>
       <c r="EG55" s="4" t="s">
         <v>562</v>
       </c>
@@ -12285,6 +12319,9 @@
       <c r="ED56" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="EE56" s="71" t="s">
+        <v>144</v>
+      </c>
       <c r="EG56" s="4" t="s">
         <v>144</v>
       </c>
@@ -12428,6 +12465,9 @@
       <c r="ED57" s="4" t="s">
         <v>194</v>
       </c>
+      <c r="EE57" s="4" t="s">
+        <v>194</v>
+      </c>
       <c r="EG57" s="4" t="s">
         <v>194</v>
       </c>
@@ -12538,6 +12578,9 @@
       <c r="ED58" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="EE58" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="EG58" s="4" t="s">
         <v>149</v>
       </c>
@@ -12642,6 +12685,9 @@
       <c r="ED59" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="EE59" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="EG59" s="4" t="s">
         <v>175</v>
       </c>
@@ -12743,6 +12789,9 @@
       </c>
       <c r="DN62" s="4" t="s">
         <v>344</v>
+      </c>
+      <c r="EE62" s="71" t="s">
+        <v>393</v>
       </c>
       <c r="EG62" s="4" t="s">
         <v>393</v>
@@ -12922,6 +12971,9 @@
       <c r="ED68" s="4" t="s">
         <v>274</v>
       </c>
+      <c r="EE68" s="71" t="s">
+        <v>1123</v>
+      </c>
       <c r="EG68" s="4" t="s">
         <v>564</v>
       </c>
@@ -12963,6 +13015,7 @@
       <c r="CU69" s="20" t="s">
         <v>252</v>
       </c>
+      <c r="EE69" s="72"/>
       <c r="EG69" s="20" t="s">
         <v>568</v>
       </c>
@@ -13041,6 +13094,9 @@
       <c r="DR72" s="4" t="s">
         <v>220</v>
       </c>
+      <c r="EE72" s="71" t="s">
+        <v>1124</v>
+      </c>
       <c r="EG72" s="4" t="s">
         <v>559</v>
       </c>
@@ -13100,6 +13156,7 @@
       <c r="A76" s="20" t="s">
         <v>125</v>
       </c>
+      <c r="EE76" s="72"/>
       <c r="FG76" s="20" t="s">
         <v>211</v>
       </c>
@@ -13141,6 +13198,9 @@
       <c r="ED77" s="4" t="s">
         <v>276</v>
       </c>
+      <c r="EE77" s="4">
+        <v>15</v>
+      </c>
       <c r="EH77" s="4" t="s">
         <v>276</v>
       </c>
@@ -13205,6 +13265,9 @@
       <c r="ED79" s="4" t="s">
         <v>271</v>
       </c>
+      <c r="EE79" s="4" t="s">
+        <v>676</v>
+      </c>
       <c r="EH79" s="4" t="s">
         <v>384</v>
       </c>
@@ -13222,1793 +13285,1744 @@
       </c>
     </row>
     <row r="80" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="O80" s="18" t="s">
-        <v>587</v>
-      </c>
-      <c r="T80" s="4" t="s">
-        <v>589</v>
+      <c r="A80" s="18" t="s">
+        <v>1013</v>
       </c>
       <c r="X80" s="18" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="81" spans="1:221" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="20" t="s">
+        <v>1015</v>
+      </c>
+      <c r="X81" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="X82" s="18" t="s">
         <v>585</v>
-      </c>
-      <c r="AE80" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="AQ80" s="4" t="s">
-        <v>595</v>
-      </c>
-      <c r="AX80" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="BA80" s="49" t="s">
-        <v>605</v>
-      </c>
-      <c r="BB80" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="CR80" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="DE80" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="ED80" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="EH80" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="FC80" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="FG80" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="HB80" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="HM80" s="4" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="81" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
-        <v>1013</v>
-      </c>
-      <c r="X81" s="18" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="82" spans="1:221" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="20" t="s">
-        <v>1015</v>
-      </c>
-      <c r="X82" s="20">
-        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>1016</v>
+      <c r="A83" s="18" t="s">
+        <v>1018</v>
       </c>
       <c r="X83" s="18" t="s">
-        <v>585</v>
+        <v>1019</v>
       </c>
     </row>
-    <row r="84" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
-        <v>1017</v>
-      </c>
-      <c r="X84" s="18" t="s">
-        <v>585</v>
+    <row r="84" spans="1:221" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="20" t="s">
+        <v>1104</v>
+      </c>
+      <c r="BD84" s="53" t="s">
+        <v>1105</v>
       </c>
     </row>
-    <row r="85" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
-        <v>1018</v>
-      </c>
-      <c r="X85" s="18" t="s">
-        <v>1019</v>
+    <row r="85" spans="1:221" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J85" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="L85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="O85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="P85" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="T85" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="V85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="W85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="X85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC85" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="AD85" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE85" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH85" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="AL85" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AM85" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AP85" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AQ85" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="AR85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AS85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AV85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AX85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="BB85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="BD85" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BT85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="CB85" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="CH85" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="CL85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="CR85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="CU85" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="DB85" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="DE85" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="DN85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="DR85" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="ED85" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="EE85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="EG85" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="EH85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="EW85" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="EZ85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="FA85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="FC85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="FG85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="FO85" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="GE85" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="HB85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="HM85" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
-    <row r="86" spans="1:221" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="20" t="s">
-        <v>1104</v>
-      </c>
-      <c r="BD86" s="53" t="s">
-        <v>1105</v>
+    <row r="86" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="O86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="P86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="T86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="V86" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="W86" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="X86" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC86" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="AD86" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE86" s="29" t="s">
+        <v>915</v>
+      </c>
+      <c r="AH86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AM86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AP86" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AQ86" s="4" t="s">
+        <v>911</v>
+      </c>
+      <c r="AR86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS86" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="AV86" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AX86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BB86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BD86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BT86" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="CB86" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="CH86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="CL86" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="CR86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="CU86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="DB86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="DE86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="DN86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="DR86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="ED86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="EE86" s="71" t="s">
+        <v>330</v>
+      </c>
+      <c r="EG86" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="EH86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="EW86" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="EZ86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="FA86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="FC86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="FG86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="FO86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="GE86" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="HB86" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="HM86" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="87" spans="1:221" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H87" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="L87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="O87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="P87" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="T87" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="V87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="W87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="X87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC87" s="5" t="s">
-        <v>910</v>
-      </c>
-      <c r="AD87" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="AE87" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="AH87" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="AL87" s="5" t="s">
+    <row r="87" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="O87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="P87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="T87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="V87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="W87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="X87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD87" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="AM87" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="AO87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="AP87" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="AQ87" s="5" t="s">
-        <v>908</v>
-      </c>
-      <c r="AR87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="AS87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="AV87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="AX87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="BB87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="BD87" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="BT87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="CB87" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="CH87" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="CL87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="CR87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="CU87" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="DB87" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="DE87" s="5" t="s">
+      <c r="AE87" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="DN87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="DR87" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="ED87" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="EG87" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="EH87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="EW87" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="EZ87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="FA87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="FC87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="FG87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="FO87" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="GE87" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="HB87" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="HM87" s="5" t="s">
-        <v>142</v>
+      <c r="AH87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AL87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AO87" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="AP87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AQ87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AR87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AS87" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AV87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AX87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="BB87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BT87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="CB87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="CH87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="CL87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="CR87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="CU87" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="DB87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="DE87" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="DN87" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="DR87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="ED87" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="EE87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="EG87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="EH87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="EW87" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="EZ87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="FA87" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="FC87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="FG87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="FO87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="GE87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="HB87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="HM87" s="4" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>142</v>
+        <v>28</v>
       </c>
       <c r="L88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="T88" s="4" t="s">
+        <v>924</v>
+      </c>
+      <c r="V88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="W88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="X88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD88" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE88" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AP88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AQ88" s="4" t="s">
+        <v>922</v>
+      </c>
+      <c r="AS88" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="O88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="P88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="T88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="V88" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="W88" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="X88" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AC88" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="AD88" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="AE88" s="29" t="s">
-        <v>915</v>
-      </c>
-      <c r="AH88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AL88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AO88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AP88" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AQ88" s="4" t="s">
-        <v>911</v>
-      </c>
-      <c r="AR88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AS88" s="4" t="s">
-        <v>318</v>
-      </c>
       <c r="AV88" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="AX88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="BB88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="BD88" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BT88" s="4" t="s">
-        <v>434</v>
+        <v>143</v>
       </c>
       <c r="CB88" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="CH88" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="CL88" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="CR88" s="4" t="s">
         <v>143</v>
       </c>
       <c r="CU88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="DB88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="DE88" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="DN88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="DR88" s="4" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="ED88" s="4" t="s">
-        <v>142</v>
+        <v>163</v>
+      </c>
+      <c r="EE88" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="EG88" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="EH88" s="4" t="s">
         <v>143</v>
       </c>
       <c r="EW88" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="EZ88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="FA88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="FC88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="FG88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="FO88" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="GE88" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="HB88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="HM88" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="L89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="O89" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD89" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE89" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AQ89" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="P89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="T89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="V89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="W89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="X89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD89" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AE89" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="AH89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AL89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AO89" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="AP89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AQ89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AR89" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="AS89" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="AV89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AX89" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="BB89" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="BD89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="BT89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="CB89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="CH89" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="CL89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="CR89" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="CU89" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="DB89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="DE89" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="DN89" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="DR89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="ED89" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="EG89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="EH89" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="EW89" s="59" t="s">
-        <v>142</v>
-      </c>
-      <c r="EZ89" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="FA89" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="FC89" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="FG89" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="FO89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="GE89" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="HB89" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="HM89" s="4" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="T90" s="4" t="s">
-        <v>924</v>
-      </c>
-      <c r="V90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="W90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="X90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AC90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AD90" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE90" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AP90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AQ90" s="4" t="s">
-        <v>922</v>
+        <v>1045</v>
+      </c>
+      <c r="AE90" s="29" t="s">
+        <v>1047</v>
       </c>
       <c r="AS90" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="AV90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="BT90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="CB90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="CL90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="CU90" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="ED90" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="EG90" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="EW90" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="GE90" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD91" s="4" t="s">
-        <v>143</v>
+        <v>1046</v>
       </c>
       <c r="AE91" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AQ91" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AS91" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="CL91" s="4" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
-    <row r="92" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>1045</v>
-      </c>
-      <c r="AE92" s="29" t="s">
-        <v>1047</v>
-      </c>
-      <c r="AS92" s="4" t="s">
-        <v>143</v>
+    <row r="92" spans="1:221" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="CB92" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="GE92" s="5" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="93" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>1046</v>
-      </c>
-      <c r="AE93" s="4" t="s">
-        <v>143</v>
+        <v>127</v>
+      </c>
+      <c r="CB93" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="GE93" s="4" t="s">
+        <v>477</v>
       </c>
     </row>
-    <row r="94" spans="1:221" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="CB94" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="GE94" s="5" t="s">
-        <v>476</v>
+    <row r="94" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="CB94" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="GE94" s="4" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="95" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="CB95" s="4" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="GE95" s="4" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="96" spans="1:221" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="CB96" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="GE96" s="4" t="s">
-        <v>478</v>
+        <v>72</v>
+      </c>
+      <c r="CU96" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="97" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="CB97" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="GE97" s="4" t="s">
-        <v>479</v>
+        <v>73</v>
+      </c>
+      <c r="CL97" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="CU97" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="EZ97" s="4" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="98" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="CU98" s="4" t="s">
-        <v>134</v>
+        <v>123</v>
+      </c>
+      <c r="BT98" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="CH98" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="EG98" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="FO98" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="CL99" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="CU99" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="EZ99" s="4" t="s">
-        <v>401</v>
+        <v>114</v>
+      </c>
+      <c r="EH99" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="HB99" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
-    <row r="100" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="BT100" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="CH100" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="EG100" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="FO100" s="4" t="s">
-        <v>174</v>
+    <row r="100" spans="1:210" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS100" s="64" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AV100" s="64" t="s">
+        <v>1091</v>
+      </c>
+      <c r="BD100" s="64" t="s">
+        <v>1108</v>
+      </c>
+      <c r="BT100" s="64" t="s">
+        <v>561</v>
+      </c>
+      <c r="CH100" s="64" t="s">
+        <v>439</v>
+      </c>
+      <c r="CL100" s="64" t="s">
+        <v>367</v>
+      </c>
+      <c r="CU100" s="64" t="s">
+        <v>251</v>
+      </c>
+      <c r="ED100" s="64" t="s">
+        <v>281</v>
+      </c>
+      <c r="EG100" s="64" t="s">
+        <v>567</v>
+      </c>
+      <c r="EH100" s="64" t="s">
+        <v>392</v>
+      </c>
+      <c r="EZ100" s="64" t="s">
+        <v>396</v>
+      </c>
+      <c r="FO100" s="64" t="s">
+        <v>447</v>
+      </c>
+      <c r="HB100" s="64" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="101" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>114</v>
+        <v>63</v>
+      </c>
+      <c r="AS101" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="AV101" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="BD101" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="BT101" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="CH101" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="CL101" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="CU101" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="ED101" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="EG101" s="4" t="s">
+        <v>562</v>
       </c>
       <c r="EH101" s="4" t="s">
-        <v>134</v>
+        <v>383</v>
+      </c>
+      <c r="EZ101" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="FO101" s="4" t="s">
+        <v>440</v>
       </c>
       <c r="HB101" s="4" t="s">
-        <v>134</v>
+        <v>407</v>
       </c>
     </row>
-    <row r="102" spans="1:210" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS102" s="64" t="s">
-        <v>1066</v>
-      </c>
-      <c r="AV102" s="64" t="s">
-        <v>1091</v>
-      </c>
-      <c r="BD102" s="64" t="s">
-        <v>1108</v>
-      </c>
-      <c r="BT102" s="64" t="s">
-        <v>561</v>
-      </c>
-      <c r="CH102" s="64" t="s">
-        <v>439</v>
-      </c>
-      <c r="CL102" s="64" t="s">
-        <v>367</v>
-      </c>
-      <c r="CU102" s="64" t="s">
-        <v>251</v>
-      </c>
-      <c r="ED102" s="64" t="s">
-        <v>281</v>
-      </c>
-      <c r="EG102" s="64" t="s">
-        <v>567</v>
-      </c>
-      <c r="EH102" s="64" t="s">
-        <v>392</v>
-      </c>
-      <c r="EZ102" s="64" t="s">
-        <v>396</v>
-      </c>
-      <c r="FO102" s="64" t="s">
-        <v>447</v>
-      </c>
-      <c r="HB102" s="64" t="s">
-        <v>413</v>
+    <row r="102" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="BD102" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="BT102" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="CH102" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="CL102" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="CU102" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="ED102" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="EG102" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="EH102" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="EZ102" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="FO102" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="HB102" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="103" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS103" s="4" t="s">
-        <v>770</v>
-      </c>
-      <c r="AV103" s="4" t="s">
-        <v>764</v>
+        <v>52</v>
       </c>
       <c r="BD103" s="4" t="s">
-        <v>772</v>
+        <v>194</v>
       </c>
       <c r="BT103" s="4" t="s">
-        <v>556</v>
+        <v>194</v>
       </c>
       <c r="CH103" s="4" t="s">
-        <v>431</v>
+        <v>194</v>
       </c>
       <c r="CL103" s="4" t="s">
-        <v>361</v>
+        <v>194</v>
       </c>
       <c r="CU103" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="ED103" s="4" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="EG103" s="4" t="s">
-        <v>562</v>
+        <v>194</v>
       </c>
       <c r="EH103" s="4" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="EZ103" s="4" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="FO103" s="4" t="s">
-        <v>440</v>
+        <v>194</v>
       </c>
       <c r="HB103" s="4" t="s">
-        <v>407</v>
+        <v>386</v>
       </c>
     </row>
     <row r="104" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="BD104" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="BT104" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="CH104" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="CL104" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="CU104" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="ED104" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="EG104" s="4" t="s">
-        <v>156</v>
+        <v>57</v>
+      </c>
+      <c r="AS104" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="AV104" s="38" t="s">
+        <v>149</v>
       </c>
       <c r="EH104" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="EZ104" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="FO104" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="HB104" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="105" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="BD105" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="BT105" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="CH105" s="4" t="s">
-        <v>194</v>
+        <v>55</v>
+      </c>
+      <c r="AS105" s="4">
+        <v>144000</v>
+      </c>
+      <c r="AV105" s="4">
+        <v>144000</v>
       </c>
       <c r="CL105" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="CU105" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="ED105" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="EG105" s="4" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="EH105" s="4" t="s">
-        <v>386</v>
+        <v>175</v>
       </c>
       <c r="EZ105" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="FO105" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="HB105" s="4" t="s">
-        <v>386</v>
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AS106" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="AV106" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="EH106" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="EZ106" s="4" t="s">
-        <v>149</v>
+      <c r="A106" s="49" t="s">
+        <v>1107</v>
+      </c>
+      <c r="BD106" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS107" s="4">
-        <v>144000</v>
-      </c>
-      <c r="AV107" s="4">
-        <v>144000</v>
-      </c>
-      <c r="CL107" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="EH107" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="EZ107" s="4" t="s">
-        <v>175</v>
+        <v>81</v>
+      </c>
+      <c r="BT107" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CH107" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CU107" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="EG107" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="FO107" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="49" t="s">
-        <v>1107</v>
-      </c>
-      <c r="BD108" s="4">
-        <v>2</v>
+      <c r="A108" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="CL108" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="EH108" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="HB108" s="4" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="109" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="BT109" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="CH109" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="CU109" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="EG109" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="FO109" s="4" t="b">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="CL109" s="4" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="110" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>111</v>
+        <v>56</v>
+      </c>
+      <c r="AS110" s="38" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AV110" s="49" t="s">
+        <v>1092</v>
+      </c>
+      <c r="BD110" s="49" t="s">
+        <v>1102</v>
+      </c>
+      <c r="BT110" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="CH110" s="4" t="s">
+        <v>438</v>
       </c>
       <c r="CL110" s="4" t="s">
-        <v>300</v>
+        <v>366</v>
+      </c>
+      <c r="CU110" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="ED110" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="EG110" s="4" t="s">
+        <v>566</v>
       </c>
       <c r="EH110" s="4" t="s">
-        <v>393</v>
+        <v>387</v>
+      </c>
+      <c r="EZ110" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="FO110" s="4" t="s">
+        <v>446</v>
       </c>
       <c r="HB110" s="4" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
-    <row r="111" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="CL111" s="4" t="s">
-        <v>371</v>
+    <row r="111" spans="1:210" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="CU111" s="20" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="112" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AS112" s="38" t="s">
-        <v>1114</v>
-      </c>
-      <c r="AV112" s="49" t="s">
-        <v>1092</v>
-      </c>
-      <c r="BD112" s="49" t="s">
-        <v>1102</v>
-      </c>
-      <c r="BT112" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="CH112" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="CL112" s="4" t="s">
-        <v>366</v>
+        <v>78</v>
       </c>
       <c r="CU112" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="ED112" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="EG112" s="4" t="s">
-        <v>566</v>
-      </c>
-      <c r="EH112" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="EZ112" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="FO112" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="HB112" s="4" t="s">
-        <v>387</v>
+        <v>247</v>
       </c>
     </row>
-    <row r="113" spans="1:210" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="CU113" s="20" t="s">
-        <v>252</v>
+    <row r="113" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="CU113" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="EH113" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="HB113" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="114" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>78</v>
+        <v>54</v>
+      </c>
+      <c r="AS114" s="38" t="s">
+        <v>1067</v>
+      </c>
+      <c r="AV114" s="49" t="s">
+        <v>1090</v>
       </c>
       <c r="CU114" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="ED114" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="EH114" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="HB114" s="4" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="115" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="CU115" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="EH115" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="HB115" s="4" t="s">
-        <v>179</v>
+        <v>255</v>
       </c>
     </row>
     <row r="116" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AS116" s="38" t="s">
-        <v>1067</v>
-      </c>
-      <c r="AV116" s="49" t="s">
-        <v>1090</v>
+        <v>76</v>
       </c>
       <c r="CU116" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="ED116" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="EH116" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="HB116" s="4" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="117" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="CU117" s="4" t="s">
-        <v>255</v>
+        <v>115</v>
+      </c>
+      <c r="AS117" s="38"/>
+      <c r="AV117" s="49" t="s">
+        <v>344</v>
+      </c>
+      <c r="EH117" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="HB117" s="4" t="s">
+        <v>393</v>
       </c>
     </row>
-    <row r="118" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="CU118" s="4" t="s">
-        <v>247</v>
+    <row r="118" spans="1:210" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="CH118" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="EZ118" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="FO118" s="5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="119" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AS119" s="38"/>
-      <c r="AV119" s="49" t="s">
-        <v>344</v>
-      </c>
-      <c r="EH119" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="HB119" s="4" t="s">
-        <v>393</v>
+        <v>118</v>
+      </c>
+      <c r="BT119" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="CH119" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="EG119" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="EZ119" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="FO119" s="4" t="s">
+        <v>441</v>
       </c>
     </row>
-    <row r="120" spans="1:210" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="CH120" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="EZ120" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="FO120" s="5" t="s">
-        <v>252</v>
+    <row r="120" spans="1:210" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="20" t="s">
+        <v>1109</v>
+      </c>
+      <c r="BD120" s="53" t="s">
+        <v>1105</v>
       </c>
     </row>
-    <row r="121" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BT121" s="4" t="s">
-        <v>557</v>
-      </c>
-      <c r="CH121" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="EG121" s="4" t="s">
-        <v>563</v>
-      </c>
-      <c r="EZ121" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="FO121" s="4" t="s">
-        <v>441</v>
+    <row r="121" spans="1:210" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS121" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AV121" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD121" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BT121" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="CH121" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="CL121" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="CU121" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="ED121" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="EG121" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="EH121" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="EZ121" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="FO121" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="HB121" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
-    <row r="122" spans="1:210" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="20" t="s">
-        <v>1109</v>
-      </c>
-      <c r="BD122" s="53" t="s">
-        <v>1105</v>
+    <row r="122" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS122" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="AV122" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="BD122" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BT122" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="CH122" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="CL122" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="CU122" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="ED122" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="EG122" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="EH122" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="EZ122" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="FO122" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="HB122" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="123" spans="1:210" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS123" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="AV123" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="BD123" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="BT123" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="CH123" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="CL123" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="CU123" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="ED123" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="EG123" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="EH123" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="EZ123" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="FO123" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="HB123" s="5" t="s">
-        <v>142</v>
+    <row r="123" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS123" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AV123" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BD123" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BT123" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="CH123" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="CL123" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="CU123" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="ED123" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="EG123" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="EH123" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="EZ123" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="FO123" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="HB123" s="4" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="124" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="AS124" s="4" t="s">
-        <v>318</v>
+        <v>141</v>
       </c>
       <c r="AV124" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="BD124" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BT124" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="CH124" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="CL124" s="4" t="s">
-        <v>363</v>
+        <v>143</v>
       </c>
       <c r="CU124" s="4" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="ED124" s="4" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="EG124" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="EH124" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="EZ124" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="FO124" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="HB124" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="125" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="AS125" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="AV125" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="BD125" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="BT125" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="CH125" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="CL125" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="CU125" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="ED125" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="EG125" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="EH125" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="EZ125" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="FO125" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="HB125" s="4" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="126" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>82</v>
+        <v>1068</v>
       </c>
       <c r="AS126" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="AV126" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="BT126" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="CL126" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="CU126" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="ED126" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="EG126" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AS127" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="CL127" s="4" t="s">
-        <v>163</v>
+        <v>79</v>
+      </c>
+      <c r="CU127" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="128" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>1068</v>
-      </c>
-      <c r="AS128" s="4" t="s">
-        <v>143</v>
+        <v>80</v>
+      </c>
+      <c r="CL128" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="CU128" s="4" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="129" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="CU129" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="EH129" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="HB129" s="4" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="130" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="CL130" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="CU130" s="4" t="s">
-        <v>256</v>
+    <row r="130" spans="1:210" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B130" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C130" s="65" t="s">
+        <v>375</v>
+      </c>
+      <c r="AT130" s="65">
+        <v>5</v>
+      </c>
+      <c r="CL130" s="65" t="s">
+        <v>134</v>
       </c>
     </row>
-    <row r="131" spans="1:210" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="EH131" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="HB131" s="4" t="s">
+    <row r="131" spans="1:210" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT131" s="13">
+        <v>5</v>
+      </c>
+      <c r="CL131" s="13" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="132" spans="1:210" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B132" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="C132" s="65" t="s">
-        <v>375</v>
+        <v>1097</v>
       </c>
       <c r="AT132" s="65">
         <v>5</v>
       </c>
-      <c r="CL132" s="65" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="133" spans="1:210" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="13" t="s">
-        <v>113</v>
+      <c r="A133" s="54" t="s">
+        <v>1098</v>
       </c>
       <c r="AT133" s="13">
         <v>5</v>
       </c>
-      <c r="CL133" s="13" t="s">
-        <v>134</v>
-      </c>
     </row>
-    <row r="134" spans="1:210" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="65" t="s">
-        <v>1097</v>
-      </c>
-      <c r="AT134" s="65">
-        <v>5</v>
+    <row r="134" spans="1:210" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="V134" s="14" t="s">
+        <v>954</v>
+      </c>
+      <c r="DD134" s="14" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="135" spans="1:210" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="54" t="s">
-        <v>1098</v>
-      </c>
-      <c r="AT135" s="13">
-        <v>5</v>
+    <row r="135" spans="1:210" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="V135" s="14" t="s">
+        <v>955</v>
+      </c>
+      <c r="DD135" s="14" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="136" spans="1:210" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="V136" s="14" t="s">
-        <v>954</v>
-      </c>
-      <c r="DD136" s="14" t="s">
-        <v>262</v>
+    <row r="136" spans="1:210" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="U136" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="AU136" s="41" t="s">
+        <v>1077</v>
+      </c>
+      <c r="FE136" s="15" t="s">
+        <v>306</v>
       </c>
     </row>
-    <row r="137" spans="1:210" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="V137" s="14" t="s">
-        <v>955</v>
-      </c>
-      <c r="DD137" s="14" t="s">
-        <v>263</v>
+    <row r="137" spans="1:210" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="U137" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU137" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="FE137" s="11" t="s">
+        <v>307</v>
       </c>
     </row>
-    <row r="138" spans="1:210" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="U138" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="AU138" s="41" t="s">
-        <v>1077</v>
-      </c>
-      <c r="FE138" s="15" t="s">
-        <v>306</v>
+    <row r="138" spans="1:210" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU138" s="42" t="s">
+        <v>1078</v>
       </c>
     </row>
-    <row r="139" spans="1:210" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="U139" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU139" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="FE139" s="11" t="s">
-        <v>307</v>
+    <row r="139" spans="1:210" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="U139" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="AU139" s="43" t="s">
+        <v>1079</v>
+      </c>
+      <c r="FE139" s="15" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="140" spans="1:210" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="AU140" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="U140" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU140" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="FE140" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="141" spans="1:210" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU141" s="42" t="s">
         <v>1078</v>
       </c>
     </row>
-    <row r="141" spans="1:210" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="U141" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="AU141" s="43" t="s">
-        <v>1079</v>
-      </c>
-      <c r="FE141" s="15" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="142" spans="1:210" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="U142" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU142" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="FE142" s="11" t="s">
-        <v>307</v>
+    <row r="142" spans="1:210" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="U142" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="AU142" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="FE142" s="15" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="143" spans="1:210" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="AU143" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="U143" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU143" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="FE143" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="144" spans="1:210" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="U144" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU144" s="42" t="s">
         <v>1078</v>
       </c>
+      <c r="FE144" s="11" t="s">
+        <v>307</v>
+      </c>
     </row>
-    <row r="144" spans="1:210" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="U144" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="AU144" s="43" t="s">
-        <v>1080</v>
-      </c>
-      <c r="FE144" s="15" t="s">
-        <v>309</v>
+    <row r="145" spans="1:171" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="66" t="s">
+        <v>940</v>
+      </c>
+      <c r="F145" s="66">
+        <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:171" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="U145" s="11" t="b">
+    <row r="146" spans="1:171" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="F146" s="2">
         <v>0</v>
       </c>
-      <c r="AU145" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="FE145" s="11" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="146" spans="1:171" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="U146" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU146" s="42" t="s">
-        <v>1078</v>
-      </c>
-      <c r="FE146" s="11" t="s">
-        <v>307</v>
+    <row r="147" spans="1:171" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="63" t="s">
+        <v>970</v>
+      </c>
+      <c r="AF147" s="63" t="s">
+        <v>972</v>
       </c>
     </row>
-    <row r="147" spans="1:171" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="66" t="s">
-        <v>940</v>
-      </c>
-      <c r="F147" s="66">
-        <v>1</v>
+    <row r="148" spans="1:171" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="6" t="s">
+        <v>962</v>
+      </c>
+      <c r="AF148" s="6" t="s">
+        <v>971</v>
       </c>
     </row>
-    <row r="148" spans="1:171" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>941</v>
-      </c>
-      <c r="F148" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:171" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="63" t="s">
-        <v>970</v>
-      </c>
-      <c r="AF149" s="63" t="s">
-        <v>972</v>
+    <row r="149" spans="1:171" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="6" t="s">
+        <v>963</v>
+      </c>
+      <c r="AF149" s="6" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="150" spans="1:171" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
-        <v>962</v>
-      </c>
-      <c r="AF150" s="6" t="s">
-        <v>971</v>
+        <v>964</v>
+      </c>
+      <c r="AF150" s="6">
+        <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:171" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="6" t="s">
-        <v>963</v>
-      </c>
-      <c r="AF151" s="6" t="s">
-        <v>578</v>
+    <row r="151" spans="1:171" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="64" t="s">
+        <v>994</v>
+      </c>
+      <c r="AW151" s="64">
+        <v>144000</v>
+      </c>
+      <c r="CE151" s="64">
+        <v>144000</v>
       </c>
     </row>
-    <row r="152" spans="1:171" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="6" t="s">
-        <v>964</v>
-      </c>
-      <c r="AF152" s="6">
+    <row r="152" spans="1:171" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="M152" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="Z152" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="AB152" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="AQ152" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="AW152" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="CE152" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="CH152" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="DR152" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="FO152" s="4" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:171" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
+        <v>993</v>
+      </c>
+      <c r="M153" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z153" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB153" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ153" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW153" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="153" spans="1:171" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="64" t="s">
-        <v>994</v>
-      </c>
-      <c r="AW153" s="64">
-        <v>144000</v>
-      </c>
-      <c r="CE153" s="64">
-        <v>144000</v>
+      <c r="CE153" s="4">
+        <v>1</v>
+      </c>
+      <c r="CH153" s="4">
+        <v>0</v>
+      </c>
+      <c r="DR153" s="4">
+        <v>0</v>
+      </c>
+      <c r="FO153" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:171" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>997</v>
-      </c>
-      <c r="M154" s="4" t="s">
-        <v>998</v>
-      </c>
-      <c r="Z154" s="4" t="s">
-        <v>998</v>
-      </c>
-      <c r="AB154" s="4" t="s">
-        <v>998</v>
-      </c>
-      <c r="AQ154" s="4" t="s">
-        <v>998</v>
-      </c>
-      <c r="AW154" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="CE154" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="CH154" s="4" t="s">
-        <v>998</v>
-      </c>
-      <c r="DR154" s="4" t="s">
-        <v>998</v>
-      </c>
-      <c r="FO154" s="4" t="s">
-        <v>998</v>
+        <v>999</v>
+      </c>
+      <c r="CE154" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:171" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>993</v>
-      </c>
-      <c r="M155" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z155" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB155" s="4">
-        <v>0</v>
-      </c>
-      <c r="AQ155" s="4">
-        <v>0</v>
-      </c>
-      <c r="AW155" s="4">
-        <v>2</v>
-      </c>
-      <c r="CE155" s="4">
+        <v>1004</v>
+      </c>
+      <c r="M155" s="4" t="s">
+        <v>909</v>
+      </c>
+      <c r="Z155" s="4" t="s">
+        <v>909</v>
+      </c>
+      <c r="AB155" s="29" t="s">
+        <v>921</v>
+      </c>
+      <c r="AQ155" s="29" t="s">
+        <v>911</v>
+      </c>
+      <c r="AW155" s="29" t="s">
+        <v>911</v>
+      </c>
+      <c r="CE155" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="CH155" s="4" t="s">
+        <v>909</v>
+      </c>
+      <c r="DR155" s="4" t="s">
+        <v>909</v>
+      </c>
+      <c r="FO155" s="4" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="156" spans="1:171" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="20" t="s">
+        <v>995</v>
+      </c>
+      <c r="M156" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="CH155" s="4">
-        <v>0</v>
-      </c>
-      <c r="DR155" s="4">
-        <v>0</v>
-      </c>
-      <c r="FO155" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:171" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="4" t="s">
-        <v>999</v>
-      </c>
-      <c r="CE156" s="4" t="b">
+      <c r="Z156" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB156" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ156" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW156" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="CE156" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="CH156" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="DR156" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="FO156" s="20" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:171" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>1004</v>
+        <v>996</v>
       </c>
       <c r="M157" s="4" t="s">
-        <v>909</v>
+        <v>981</v>
       </c>
       <c r="Z157" s="4" t="s">
-        <v>909</v>
+        <v>991</v>
       </c>
       <c r="AB157" s="29" t="s">
-        <v>921</v>
+        <v>1038</v>
       </c>
       <c r="AQ157" s="29" t="s">
-        <v>911</v>
-      </c>
-      <c r="AW157" s="29" t="s">
-        <v>911</v>
+        <v>1059</v>
+      </c>
+      <c r="AW157" s="38" t="s">
+        <v>1071</v>
       </c>
       <c r="CE157" s="4" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="CH157" s="4" t="s">
-        <v>909</v>
+        <v>437</v>
       </c>
       <c r="DR157" s="4" t="s">
-        <v>909</v>
+        <v>217</v>
       </c>
       <c r="FO157" s="4" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="158" spans="1:171" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="20" t="s">
-        <v>995</v>
-      </c>
-      <c r="M158" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z158" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB158" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ158" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="AW158" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="CE158" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="CH158" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="DR158" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="FO158" s="20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:171" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="4" t="s">
-        <v>996</v>
-      </c>
-      <c r="M159" s="4" t="s">
-        <v>981</v>
-      </c>
-      <c r="Z159" s="4" t="s">
-        <v>991</v>
-      </c>
-      <c r="AB159" s="29" t="s">
-        <v>1038</v>
-      </c>
-      <c r="AQ159" s="29" t="s">
-        <v>1059</v>
-      </c>
-      <c r="AW159" s="38" t="s">
-        <v>1071</v>
-      </c>
-      <c r="CE159" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="CH159" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="DR159" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="FO159" s="4" t="s">
         <v>437</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B1:IA159">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B1:IA157">
     <sortCondition ref="B9:IA9"/>
   </sortState>
-  <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="A147">
-    <cfRule type="duplicateValues" dxfId="23" priority="13"/>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <conditionalFormatting sqref="A145">
+    <cfRule type="duplicateValues" dxfId="22" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A148">
-    <cfRule type="duplicateValues" dxfId="22" priority="12"/>
+  <conditionalFormatting sqref="A146">
+    <cfRule type="duplicateValues" dxfId="21" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:A41">
-    <cfRule type="duplicateValues" dxfId="21" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A155:A157">
-    <cfRule type="duplicateValues" dxfId="20" priority="8"/>
+  <conditionalFormatting sqref="A153:A155">
+    <cfRule type="duplicateValues" dxfId="19" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A153:A154">
-    <cfRule type="duplicateValues" dxfId="19" priority="7"/>
+  <conditionalFormatting sqref="A151:A152">
+    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A158">
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+  <conditionalFormatting sqref="A156">
+    <cfRule type="duplicateValues" dxfId="17" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A159">
-    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
+  <conditionalFormatting sqref="A157">
+    <cfRule type="duplicateValues" dxfId="16" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1">
     <cfRule type="expression" dxfId="15" priority="24">
@@ -15016,11 +15030,11 @@
     </cfRule>
     <cfRule type="duplicateValues" dxfId="14" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42:A146 A1:A39">
-    <cfRule type="duplicateValues" dxfId="13" priority="108"/>
+  <conditionalFormatting sqref="A147:A150">
+    <cfRule type="duplicateValues" dxfId="13" priority="110"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A149:A152">
-    <cfRule type="duplicateValues" dxfId="12" priority="110"/>
+  <conditionalFormatting sqref="A42:A144 A1:A39">
+    <cfRule type="duplicateValues" dxfId="0" priority="112"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -37577,40 +37591,40 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="FD1">
-    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="FE1">
-    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO1:AP1">
-    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN1:FP1">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL1:FM1">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="FR1">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="FS1">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF1:FK1">
-    <cfRule type="duplicateValues" dxfId="4" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="FQ1">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AN1 AQ1:FC1">
-    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A98">
-    <cfRule type="expression" dxfId="1" priority="94">
+    <cfRule type="expression" dxfId="2" priority="94">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="95"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>